<commit_message>
Find A Ride test case updated
</commit_message>
<xml_diff>
--- a/TestData/Sharecar data.xlsx
+++ b/TestData/Sharecar data.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27531"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27628"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Selenium\ShareCar\TestData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D451E95D-B786-44CC-8227-702C799B0AC8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3F419EF5-ABCE-4F16-806A-3A63225B60C1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="21795" windowHeight="12975" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3525" yWindow="3472" windowWidth="16200" windowHeight="9308" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="2" r:id="rId1"/>
@@ -153,7 +153,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="1" applyBorder="1"/>
@@ -165,7 +165,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="20" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="2">
@@ -450,8 +449,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{063145DA-9334-46AB-962F-889FB364BC63}">
   <dimension ref="A1:G2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A3" sqref="A3:XFD3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -521,8 +520,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{87DD51B8-45CE-4D71-8C79-511650FE34E2}">
   <dimension ref="A1:J2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D3" sqref="D3"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -581,19 +580,19 @@
       <c r="C2" s="3">
         <v>0.2361111111111111</v>
       </c>
-      <c r="D2" s="7">
+      <c r="D2" s="1">
         <v>1234</v>
       </c>
       <c r="E2" s="1">
         <v>1220</v>
       </c>
-      <c r="F2" s="7">
+      <c r="F2" s="1">
         <v>2589</v>
       </c>
       <c r="G2" s="4">
         <v>45527</v>
       </c>
-      <c r="H2" s="8">
+      <c r="H2" s="7">
         <v>0.34027777777777779</v>
       </c>
       <c r="I2">

</xml_diff>